<commit_message>
added Individaul Drawings of GUI Class
</commit_message>
<xml_diff>
--- a/SQLFiles/DataBase Design.xlsx
+++ b/SQLFiles/DataBase Design.xlsx
@@ -4,18 +4,21 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="105" windowWidth="27795" windowHeight="12600"/>
+    <workbookView xWindow="480" yWindow="105" windowWidth="14880" windowHeight="8610"/>
   </bookViews>
   <sheets>
     <sheet name="Design 1" sheetId="1" r:id="rId1"/>
     <sheet name="Design 2" sheetId="3" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Design 1'!$A$2:$I$24</definedName>
+  </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="41">
   <si>
     <t>Painters</t>
   </si>
@@ -27,9 +30,6 @@
   </si>
   <si>
     <t>Fashionability</t>
-  </si>
-  <si>
-    <t>PainterID (Main Key)</t>
   </si>
   <si>
     <t>------------</t>
@@ -646,387 +646,387 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C2:J24"/>
+  <dimension ref="A2:H24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="29.85546875" customWidth="1"/>
-    <col min="6" max="6" width="17.5703125" customWidth="1"/>
-    <col min="7" max="7" width="26.42578125" style="2" customWidth="1"/>
-    <col min="9" max="9" width="31.42578125" customWidth="1"/>
-    <col min="10" max="10" width="9.28515625" customWidth="1"/>
+    <col min="2" max="2" width="29.85546875" customWidth="1"/>
+    <col min="4" max="4" width="17.5703125" customWidth="1"/>
+    <col min="5" max="5" width="26.42578125" style="2" customWidth="1"/>
+    <col min="7" max="7" width="31.42578125" customWidth="1"/>
+    <col min="8" max="8" width="9.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C3" s="7"/>
-      <c r="D3" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="E3" s="1"/>
+    <row r="2" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="7"/>
+      <c r="B3" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="5" t="s">
+        <v>39</v>
+      </c>
       <c r="F3" s="1"/>
       <c r="G3" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="H3" s="7"/>
+    </row>
+    <row r="4" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A4" s="7"/>
+      <c r="B4" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="H3" s="1"/>
-      <c r="I3" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="J3" s="7"/>
-    </row>
-    <row r="4" spans="3:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="C4" s="7"/>
-      <c r="D4" s="9" t="s">
+      <c r="C4" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="D4" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G4" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="H4" s="7"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="17" t="s">
-        <v>31</v>
-      </c>
-      <c r="G4" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="H4" s="3" t="s">
+      <c r="C5" s="1"/>
+      <c r="D5" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="F5" s="1"/>
+      <c r="G5" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="I4" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="J4" s="7"/>
-    </row>
-    <row r="5" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C5" s="10" t="s">
+      <c r="H5" s="11" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" s="1"/>
+      <c r="D6" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F6" s="1"/>
+      <c r="G6" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="H6" s="18" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7" s="1"/>
+      <c r="D7" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="F7" s="1"/>
+      <c r="G7" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="H7" s="11" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="D5" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="E5" s="1"/>
-      <c r="F5" s="10" t="s">
+      <c r="B8" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="H8" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="G5" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="H5" s="1"/>
-      <c r="I5" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="J5" s="11" t="s">
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="15" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="6" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C6" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="E6" s="1"/>
-      <c r="F6" s="10" t="s">
+      <c r="B9" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="H9" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="G6" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="H6" s="1"/>
-      <c r="I6" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="J6" s="18" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="7" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C7" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="E7" s="1"/>
-      <c r="F7" s="10" t="s">
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="G7" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="H7" s="1"/>
-      <c r="I7" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="J7" s="11" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="8" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C8" s="15" t="s">
+      <c r="B10" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="H10" s="12" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" s="7"/>
+      <c r="D11" s="7"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="H11" s="11" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C12" s="7"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="7"/>
+      <c r="G12" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="H12" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="D8" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="E8" s="7"/>
-      <c r="F8" s="7"/>
-      <c r="G8" s="1"/>
-      <c r="H8" s="7"/>
-      <c r="I8" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="J8" s="15" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="9" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C9" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="D9" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E9" s="7"/>
-      <c r="F9" s="7"/>
-      <c r="G9" s="1"/>
-      <c r="H9" s="7"/>
-      <c r="I9" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="J9" s="16" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="10" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C10" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="D10" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E10" s="7"/>
-      <c r="F10" s="7"/>
-      <c r="G10" s="1"/>
-      <c r="H10" s="7"/>
-      <c r="I10" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="J10" s="12" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="11" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C11" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="D11" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E11" s="7"/>
-      <c r="F11" s="7"/>
-      <c r="G11" s="1"/>
-      <c r="H11" s="7"/>
-      <c r="I11" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="J11" s="11" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="12" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C12" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="D12" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E12" s="7"/>
-      <c r="F12" s="7"/>
-      <c r="G12" s="1"/>
-      <c r="H12" s="7"/>
-      <c r="I12" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="J12" s="13" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="13" spans="3:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="7"/>
+      <c r="B13" s="7"/>
       <c r="C13" s="7"/>
       <c r="D13" s="7"/>
-      <c r="E13" s="7"/>
+      <c r="E13" s="1"/>
       <c r="F13" s="7"/>
-      <c r="G13" s="1"/>
-      <c r="H13" s="7"/>
-      <c r="I13" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="J13" s="11" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="14" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="G13" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H13" s="11" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="7"/>
+      <c r="B14" s="7"/>
       <c r="C14" s="7"/>
       <c r="D14" s="7"/>
-      <c r="E14" s="7"/>
+      <c r="E14" s="1"/>
       <c r="F14" s="7"/>
-      <c r="G14" s="1"/>
-      <c r="H14" s="7"/>
-      <c r="I14" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="J14" s="12" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="15" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="G14" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="H14" s="12" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="7"/>
+      <c r="B15" s="7"/>
       <c r="C15" s="7"/>
       <c r="D15" s="7"/>
-      <c r="E15" s="7"/>
+      <c r="E15" s="1"/>
       <c r="F15" s="7"/>
-      <c r="G15" s="1"/>
-      <c r="H15" s="7"/>
-      <c r="I15" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="J15" s="16" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="16" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="G15" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="H15" s="16" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="7"/>
+      <c r="B16" s="7"/>
       <c r="C16" s="7"/>
       <c r="D16" s="7"/>
-      <c r="E16" s="7"/>
+      <c r="E16" s="1"/>
       <c r="F16" s="7"/>
-      <c r="G16" s="1"/>
-      <c r="H16" s="7"/>
-      <c r="I16" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="J16" s="15" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="17" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="G16" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="H16" s="15" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="7"/>
+      <c r="B17" s="7"/>
       <c r="C17" s="7"/>
       <c r="D17" s="7"/>
-      <c r="E17" s="7"/>
+      <c r="E17" s="1"/>
       <c r="F17" s="7"/>
-      <c r="G17" s="1"/>
-      <c r="H17" s="7"/>
-      <c r="I17" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="J17" s="16" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="18" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="G17" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="H17" s="16" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="7"/>
+      <c r="B18" s="7"/>
       <c r="C18" s="7"/>
       <c r="D18" s="7"/>
-      <c r="E18" s="7"/>
+      <c r="E18" s="1"/>
       <c r="F18" s="7"/>
-      <c r="G18" s="1"/>
-      <c r="H18" s="7"/>
-      <c r="I18" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="J18" s="19" t="s">
+      <c r="G18" s="6" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="19" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="H18" s="19" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="7"/>
+      <c r="B19" s="7"/>
       <c r="C19" s="7"/>
       <c r="D19" s="7"/>
-      <c r="E19" s="7"/>
+      <c r="E19" s="1"/>
       <c r="F19" s="7"/>
-      <c r="G19" s="1"/>
-      <c r="H19" s="7"/>
-      <c r="I19" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="J19" s="14" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="20" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="G19" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="H19" s="14" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="7"/>
+      <c r="B20" s="7"/>
       <c r="C20" s="7"/>
       <c r="D20" s="7"/>
-      <c r="E20" s="7"/>
+      <c r="E20" s="1"/>
       <c r="F20" s="7"/>
-      <c r="G20" s="1"/>
-      <c r="H20" s="7"/>
-      <c r="I20" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="J20" s="12" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="21" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="G20" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="H20" s="12" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="7"/>
+      <c r="B21" s="7"/>
       <c r="C21" s="7"/>
       <c r="D21" s="7"/>
-      <c r="E21" s="7"/>
+      <c r="E21" s="1"/>
       <c r="F21" s="7"/>
-      <c r="G21" s="1"/>
-      <c r="H21" s="7"/>
-      <c r="I21" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="J21" s="12" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="22" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="G21" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="H21" s="12" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" s="7"/>
+      <c r="B22" s="7"/>
       <c r="C22" s="7"/>
       <c r="D22" s="7"/>
-      <c r="E22" s="7"/>
+      <c r="E22" s="1"/>
       <c r="F22" s="7"/>
-      <c r="G22" s="1"/>
-      <c r="H22" s="7"/>
-      <c r="I22" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="J22" s="15" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="23" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="G22" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="H22" s="15" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" s="7"/>
+      <c r="B23" s="7"/>
       <c r="C23" s="7"/>
       <c r="D23" s="7"/>
-      <c r="E23" s="7"/>
+      <c r="E23" s="1"/>
       <c r="F23" s="7"/>
-      <c r="G23" s="1"/>
-      <c r="H23" s="7"/>
-      <c r="I23" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="J23" s="19" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="24" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="G23" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="H23" s="19" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" s="7"/>
+      <c r="B24" s="7"/>
       <c r="C24" s="7"/>
       <c r="D24" s="7"/>
-      <c r="E24" s="7"/>
+      <c r="E24" s="1"/>
       <c r="F24" s="7"/>
-      <c r="G24" s="1"/>
-      <c r="H24" s="7"/>
-      <c r="I24" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="J24" s="19" t="s">
-        <v>36</v>
+      <c r="G24" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="H24" s="19" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1048,7 +1048,7 @@
     <row r="2" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="5" t="s">
@@ -1056,7 +1056,7 @@
       </c>
       <c r="E3" s="1"/>
       <c r="F3" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.25">
@@ -1087,7 +1087,7 @@
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B6" s="6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="6" t="s">
@@ -1095,130 +1095,130 @@
       </c>
       <c r="E6" s="1"/>
       <c r="F6" s="6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B7" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C7" s="1"/>
       <c r="E7" s="1"/>
       <c r="F7" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B8" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D8" s="2"/>
       <c r="F8" s="6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B9" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D9" s="2"/>
       <c r="F9" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B10" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D10" s="2"/>
       <c r="F10" s="6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B11" s="6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D11" s="2"/>
       <c r="F11" s="6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B12" s="6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D12" s="2"/>
       <c r="F12" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B13" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D13" s="2"/>
       <c r="F13" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.25">
       <c r="D14" s="2"/>
       <c r="F14" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.25">
       <c r="D15" s="2"/>
       <c r="F15" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="16" spans="2:6" x14ac:dyDescent="0.25">
       <c r="D16" s="2"/>
       <c r="F16" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="17" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D17" s="2"/>
       <c r="F17" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="18" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D18" s="2"/>
       <c r="F18" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="19" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D19" s="2"/>
       <c r="F19" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="20" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D20" s="2"/>
       <c r="F20" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="21" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D21" s="2"/>
       <c r="F21" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="22" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D22" s="2"/>
       <c r="F22" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="23" spans="4:6" x14ac:dyDescent="0.25">
       <c r="F23" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
SQL Source and demo added to SQL file folder
Need to install SQL for it to work
</commit_message>
<xml_diff>
--- a/SQLFiles/DataBase Design.xlsx
+++ b/SQLFiles/DataBase Design.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="42">
   <si>
     <t>Painters</t>
   </si>
@@ -141,6 +141,9 @@
   </si>
   <si>
     <t>ArtistID (Main Key)</t>
+  </si>
+  <si>
+    <t>Width</t>
   </si>
 </sst>
 </file>
@@ -648,8 +651,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:H24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -723,8 +726,8 @@
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="13" t="s">
-        <v>33</v>
+      <c r="A6" s="18" t="s">
+        <v>34</v>
       </c>
       <c r="B6" s="6" t="s">
         <v>23</v>
@@ -796,7 +799,7 @@
       <c r="E9" s="1"/>
       <c r="F9" s="7"/>
       <c r="G9" s="6" t="s">
-        <v>8</v>
+        <v>41</v>
       </c>
       <c r="H9" s="16" t="s">
         <v>32</v>
@@ -807,7 +810,7 @@
         <v>32</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>8</v>
+        <v>41</v>
       </c>
       <c r="C10" s="7"/>
       <c r="D10" s="7"/>

</xml_diff>